<commit_message>
will added some notes 2
</commit_message>
<xml_diff>
--- a/LCDataDictionary.xlsx
+++ b/LCDataDictionary.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27907"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Will/msan/distributed/teamsparkling/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060"/>
+    <workbookView xWindow="1620" yWindow="840" windowWidth="26320" windowHeight="16280"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -13,11 +18,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">browseNotes!$A$1:$B$89</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$B$57</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">LoanStats!$A$1:$D$57</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">RejectStats!$A$1:$B$10</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="311">
   <si>
     <t>id</t>
   </si>
@@ -915,6 +923,51 @@
   </si>
   <si>
     <t>total_cu_tl</t>
+  </si>
+  <si>
+    <t>Engineer</t>
+  </si>
+  <si>
+    <t>Drop</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Reason For Action</t>
+  </si>
+  <si>
+    <t>What is this?</t>
+  </si>
+  <si>
+    <t>Regex??</t>
+  </si>
+  <si>
+    <t>Combine with last_fico for some sort of change in FICO</t>
+  </si>
+  <si>
+    <t>Investigate number of OTHER</t>
+  </si>
+  <si>
+    <t>not known at loan origination</t>
+  </si>
+  <si>
+    <t>RESPONSE</t>
+  </si>
+  <si>
+    <t>The response variable.</t>
+  </si>
+  <si>
+    <t>regex??</t>
+  </si>
+  <si>
+    <t>useless</t>
+  </si>
+  <si>
+    <t>If not verified do we use status?</t>
+  </si>
+  <si>
+    <t>Mulitcolinearity</t>
   </si>
 </sst>
 </file>
@@ -1959,735 +2012,1006 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:M81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A73" sqref="A73:XFD73"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="196.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="118.83203125" style="6" customWidth="1"/>
-    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="196.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="118.83203125" style="6" customWidth="1"/>
+    <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="16" t="s">
         <v>100</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="4" customFormat="1">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="1" t="s">
         <v>242</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:4" s="4" customFormat="1">
-      <c r="A3" s="3" t="s">
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="B4" s="9"/>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1">
-      <c r="A4" s="7" t="s">
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1">
-      <c r="A5" s="7" t="s">
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>253</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" s="4" customFormat="1">
-      <c r="A6" s="7" t="s">
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B8" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:4" s="4" customFormat="1">
-      <c r="A7" s="3" t="s">
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:4" s="4" customFormat="1">
-      <c r="A8" s="3" t="s">
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:4" s="4" customFormat="1" ht="18" customHeight="1">
-      <c r="A9" s="3" t="s">
+      <c r="E10" s="5"/>
+    </row>
+    <row r="11" spans="1:6" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B11" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:4" s="4" customFormat="1">
-      <c r="A10" s="3" t="s">
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="14" customHeight="1">
-      <c r="A11" s="7" t="s">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="1:4" s="4" customFormat="1">
-      <c r="A12" s="3" t="s">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" s="4" customFormat="1">
-      <c r="A13" s="3" t="s">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="5"/>
-    </row>
-    <row r="14" spans="1:4" s="4" customFormat="1">
-      <c r="A14" s="3" t="s">
+      <c r="E15" s="25"/>
+    </row>
+    <row r="16" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B16" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C14" s="5"/>
-    </row>
-    <row r="15" spans="1:4" s="4" customFormat="1">
-      <c r="A15" s="7" t="s">
+      <c r="E16" s="25"/>
+    </row>
+    <row r="17" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B17" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>261</v>
       </c>
-      <c r="C15" s="25"/>
-    </row>
-    <row r="16" spans="1:4" s="4" customFormat="1">
-      <c r="A16" s="7" t="s">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" s="4" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B18" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C16" s="25"/>
-    </row>
-    <row r="17" spans="1:3" s="4" customFormat="1">
-      <c r="A17" s="3" t="s">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" s="4" customFormat="1" ht="14" customHeight="1">
-      <c r="A18" s="3" t="s">
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C18" s="5"/>
-    </row>
-    <row r="19" spans="1:3" s="4" customFormat="1">
-      <c r="A19" s="3" t="s">
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="5"/>
-    </row>
-    <row r="20" spans="1:3" s="4" customFormat="1">
-      <c r="A20" s="3" t="s">
+      <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B22" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C20" s="5"/>
-    </row>
-    <row r="21" spans="1:3" s="4" customFormat="1">
-      <c r="A21" s="3" t="s">
+      <c r="E22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C21" s="5"/>
-    </row>
-    <row r="22" spans="1:3" s="4" customFormat="1">
-      <c r="A22" s="3" t="s">
+      <c r="E23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="9" t="s">
+        <v>279</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:3" s="4" customFormat="1">
-      <c r="A23" s="3" t="s">
+      <c r="E25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9" t="s">
+        <v>290</v>
+      </c>
+      <c r="E26" s="5"/>
+    </row>
+    <row r="27" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="E27" s="5"/>
+    </row>
+    <row r="28" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="24" spans="1:3" s="4" customFormat="1">
-      <c r="A24" s="3" t="s">
+      <c r="E28" s="5"/>
+    </row>
+    <row r="29" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="5"/>
-    </row>
-    <row r="25" spans="1:3" s="4" customFormat="1">
-      <c r="A25" s="3" t="s">
+      <c r="E29" s="25"/>
+    </row>
+    <row r="30" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="5"/>
-    </row>
-    <row r="26" spans="1:3" s="4" customFormat="1">
-      <c r="A26" s="7" t="s">
+      <c r="E30" s="25"/>
+    </row>
+    <row r="31" spans="1:5" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C26" s="5"/>
-    </row>
-    <row r="27" spans="1:3" s="4" customFormat="1">
-      <c r="A27" s="3" t="s">
+      <c r="E31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="C27" s="5"/>
-    </row>
-    <row r="28" spans="1:3" s="4" customFormat="1">
-      <c r="A28" s="3" t="s">
+      <c r="E32" s="5"/>
+    </row>
+    <row r="33" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="C28" s="5"/>
-    </row>
-    <row r="29" spans="1:3" s="4" customFormat="1">
-      <c r="A29" s="7" t="s">
+      <c r="E33" s="5"/>
+    </row>
+    <row r="34" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B34" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>264</v>
       </c>
-      <c r="C29" s="25"/>
-    </row>
-    <row r="30" spans="1:3" s="4" customFormat="1">
-      <c r="A30" s="7" t="s">
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B35" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C30" s="25"/>
-    </row>
-    <row r="31" spans="1:3" s="4" customFormat="1" ht="18" customHeight="1">
-      <c r="A31" s="3" t="s">
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B36" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="5"/>
-    </row>
-    <row r="32" spans="1:3" s="4" customFormat="1">
-      <c r="A32" s="3" t="s">
+      <c r="E36" s="5"/>
+    </row>
+    <row r="37" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B37" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C32" s="5"/>
-    </row>
-    <row r="33" spans="1:11" s="4" customFormat="1">
-      <c r="A33" s="3" t="s">
+      <c r="E37" s="5"/>
+      <c r="K37" s="10"/>
+      <c r="L37" s="11"/>
+    </row>
+    <row r="38" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="5"/>
-    </row>
-    <row r="34" spans="1:11" s="4" customFormat="1">
-      <c r="A34" s="3" t="s">
+      <c r="E38" s="5"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B39" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="5"/>
-    </row>
-    <row r="35" spans="1:11" s="4" customFormat="1">
-      <c r="A35" s="3" t="s">
+      <c r="F39" s="4"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A40" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9" t="s">
+        <v>286</v>
+      </c>
+      <c r="F40" s="4"/>
+    </row>
+    <row r="41" spans="1:13" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="5"/>
-    </row>
-    <row r="36" spans="1:11" s="4" customFormat="1">
-      <c r="A36" s="3" t="s">
+      <c r="F41" s="4"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C36" s="5"/>
-    </row>
-    <row r="37" spans="1:11" s="4" customFormat="1">
-      <c r="A37" s="8" t="s">
+      <c r="F42" s="4"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A43" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C37" s="5"/>
-      <c r="I37" s="10"/>
-      <c r="J37" s="11"/>
-    </row>
-    <row r="38" spans="1:11" s="4" customFormat="1">
-      <c r="A38" s="3" t="s">
+      <c r="F43" s="4"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C38" s="5"/>
-    </row>
-    <row r="39" spans="1:11">
-      <c r="A39" s="3" t="s">
+      <c r="F44" s="4"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A45" s="9" t="s">
+        <v>275</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="C45" s="9"/>
+      <c r="D45" s="9" t="s">
+        <v>276</v>
+      </c>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B46" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:11">
-      <c r="A40" s="3" t="s">
+      <c r="F46" s="4"/>
+      <c r="K46" s="10"/>
+      <c r="L46" s="11"/>
+      <c r="M46" s="11"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B47" s="3"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:11" ht="16" customHeight="1">
-      <c r="A41" s="3" t="s">
+      <c r="F47" s="4"/>
+      <c r="K47" s="10"/>
+      <c r="L47" s="11"/>
+      <c r="M47" s="11"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A48" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="F48" s="4"/>
+      <c r="K48" s="12"/>
+      <c r="L48" s="11"/>
+      <c r="M48" s="11"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
+      <c r="D49" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="F49" s="4"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="9" t="s">
+        <v>273</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="9"/>
+      <c r="D50" s="9" t="s">
+        <v>274</v>
+      </c>
+      <c r="F50" s="4"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="F51" s="4"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
+        <v>281</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="F52" s="4"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9" t="s">
+        <v>284</v>
+      </c>
+      <c r="F53" s="4"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B54" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D41" s="4"/>
-    </row>
-    <row r="42" spans="1:11">
-      <c r="A42" s="3" t="s">
+      <c r="F54" s="4"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B55" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="D42" s="4"/>
-    </row>
-    <row r="43" spans="1:11" ht="28">
-      <c r="A43" s="3" t="s">
+      <c r="F55" s="4"/>
+    </row>
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B56" s="3"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="D43" s="4"/>
-    </row>
-    <row r="44" spans="1:11">
-      <c r="A44" s="3" t="s">
+      <c r="F56" s="4"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B57" s="3"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="D44" s="4"/>
-    </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="3" t="s">
+      <c r="F57" s="4"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B58" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D58" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="D45" s="4"/>
-    </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="3" t="s">
+      <c r="F58" s="4"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B59" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D59" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D46" s="4"/>
-      <c r="I46" s="10"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-    </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="7" t="s">
+      <c r="F59" s="4"/>
+    </row>
+    <row r="60" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B60" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="C60" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="D60" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D47" s="4"/>
-      <c r="I47" s="10"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-    </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="3" t="s">
+      <c r="F60" s="4"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="D48" s="4"/>
-      <c r="I48" s="12"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-    </row>
-    <row r="49" spans="1:4">
-      <c r="A49" s="3" t="s">
+      <c r="F61" s="4"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D49" s="4"/>
-    </row>
-    <row r="50" spans="1:4">
-      <c r="A50" s="3" t="s">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="D50" s="4"/>
-    </row>
-    <row r="51" spans="1:4">
-      <c r="A51" s="3" t="s">
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B64" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D51" s="4"/>
-    </row>
-    <row r="52" spans="1:4">
-      <c r="A52" s="3" t="s">
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B65" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D52" s="4"/>
-    </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="3" t="s">
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" s="9"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B67" s="9"/>
+      <c r="C67" s="9"/>
+      <c r="D67" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B68" s="3"/>
+      <c r="C68" s="3"/>
+      <c r="D68" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D53" s="4"/>
-    </row>
-    <row r="54" spans="1:4">
-      <c r="A54" s="3" t="s">
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="B69" s="9"/>
+      <c r="C69" s="9"/>
+      <c r="D69" s="9" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="B70" s="9"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B71" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="1:4">
-      <c r="A55" s="3" t="s">
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B72" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="D55" s="4"/>
-    </row>
-    <row r="56" spans="1:4">
-      <c r="A56" s="3" t="s">
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B73" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D73" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D56" s="4"/>
-    </row>
-    <row r="57" spans="1:4">
-      <c r="A57" s="3" t="s">
+      <c r="E73"/>
+      <c r="H73" s="6"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B74" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D74" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D57" s="4"/>
-    </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="3" t="s">
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B75" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D75" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D58" s="4"/>
-    </row>
-    <row r="59" spans="1:4">
-      <c r="A59" s="3" t="s">
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="B76" s="9"/>
+      <c r="C76" s="9"/>
+      <c r="D76" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B77" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D77" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D59" s="4"/>
-    </row>
-    <row r="60" spans="1:4" s="6" customFormat="1">
-      <c r="A60" s="7" t="s">
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="B60" s="7" t="s">
+      <c r="B78" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C78" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="D78" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="D60" s="4"/>
-    </row>
-    <row r="61" spans="1:4">
-      <c r="A61" s="18" t="s">
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="18" t="s">
         <v>248</v>
       </c>
-      <c r="B61" s="18" t="s">
+      <c r="B79" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>310</v>
+      </c>
+      <c r="D79" s="18" t="s">
         <v>247</v>
       </c>
-      <c r="D61" s="4"/>
-    </row>
-    <row r="62" spans="1:4">
-      <c r="A62" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="9" t="s">
-        <v>269</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
-      <c r="A64" s="9" t="s">
-        <v>271</v>
-      </c>
-      <c r="B64" s="9" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6">
-      <c r="A65" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="B65" s="9" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6">
-      <c r="A66" s="9" t="s">
-        <v>275</v>
-      </c>
-      <c r="B66" s="9" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6">
-      <c r="A67" s="9" t="s">
-        <v>277</v>
-      </c>
-      <c r="B67" s="9" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6">
-      <c r="A68" s="9" t="s">
-        <v>279</v>
-      </c>
-      <c r="B68" s="9" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6">
-      <c r="A69" s="9" t="s">
-        <v>281</v>
-      </c>
-      <c r="B69" s="9" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6">
-      <c r="A70" s="9" t="s">
-        <v>283</v>
-      </c>
-      <c r="B70" s="9" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6">
-      <c r="A71" s="9" t="s">
-        <v>285</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6">
-      <c r="A72" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6">
-      <c r="A73" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="C73"/>
-      <c r="F73" s="6"/>
-    </row>
-    <row r="74" spans="1:6">
-      <c r="A74" s="9" t="s">
-        <v>289</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6">
-      <c r="A75" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="B75" s="9" t="s">
-        <v>294</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6">
-      <c r="A76" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="B76" s="9" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6">
-      <c r="A77" s="9" t="s">
-        <v>293</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6">
-      <c r="A78" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="B78" s="9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6">
-      <c r="A79" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="B79" s="9" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2">
-      <c r="B81" s="13" t="s">
+    </row>
+    <row r="81" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D81" s="13" t="s">
         <v>169</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B57">
-    <sortState ref="A2:B61">
-      <sortCondition ref="A1:A61"/>
+  <autoFilter ref="A1:D57">
+    <sortState ref="A2:D79">
+      <sortCondition ref="A1:A79"/>
     </sortState>
   </autoFilter>
   <sortState ref="A2:B101">
@@ -2695,11 +3019,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="64" orientation="portrait" verticalDpi="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2712,14 +3031,14 @@
       <selection pane="bottomLeft" activeCell="A87" sqref="A87:XFD87"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" customWidth="1"/>
     <col min="2" max="2" width="235.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="235.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
         <v>220</v>
       </c>
@@ -2727,7 +3046,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>184</v>
       </c>
@@ -2738,7 +3057,7 @@
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>192</v>
       </c>
@@ -2749,7 +3068,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>193</v>
       </c>
@@ -2760,7 +3079,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>191</v>
       </c>
@@ -2771,7 +3090,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" s="6" customFormat="1">
+    <row r="6" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>255</v>
       </c>
@@ -2779,7 +3098,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>181</v>
       </c>
@@ -2789,7 +3108,7 @@
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" s="6" customFormat="1">
+    <row r="8" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>253</v>
       </c>
@@ -2798,7 +3117,7 @@
       </c>
       <c r="D8"/>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>115</v>
       </c>
@@ -2808,7 +3127,7 @@
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>194</v>
       </c>
@@ -2819,7 +3138,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>196</v>
       </c>
@@ -2830,7 +3149,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>106</v>
       </c>
@@ -2840,7 +3159,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>107</v>
       </c>
@@ -2850,7 +3169,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>188</v>
       </c>
@@ -2861,7 +3180,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>197</v>
       </c>
@@ -2872,7 +3191,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>198</v>
       </c>
@@ -2883,7 +3202,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>18</v>
       </c>
@@ -2894,7 +3213,7 @@
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>22</v>
       </c>
@@ -2905,7 +3224,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" s="6" customFormat="1">
+    <row r="19" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>256</v>
       </c>
@@ -2914,7 +3233,7 @@
       </c>
       <c r="D19"/>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>199</v>
       </c>
@@ -2925,7 +3244,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>240</v>
       </c>
@@ -2935,7 +3254,7 @@
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>167</v>
       </c>
@@ -2946,7 +3265,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="9" t="s">
         <v>178</v>
       </c>
@@ -2957,7 +3276,7 @@
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="9" t="s">
         <v>186</v>
       </c>
@@ -2968,7 +3287,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="9" t="s">
         <v>174</v>
       </c>
@@ -2979,7 +3298,7 @@
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>201</v>
       </c>
@@ -2990,7 +3309,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="9" t="s">
         <v>200</v>
       </c>
@@ -3001,7 +3320,7 @@
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>172</v>
       </c>
@@ -3012,7 +3331,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="9" t="s">
         <v>8</v>
       </c>
@@ -3023,7 +3342,7 @@
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>180</v>
       </c>
@@ -3034,7 +3353,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>0</v>
       </c>
@@ -3045,7 +3364,7 @@
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>162</v>
       </c>
@@ -3055,7 +3374,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>217</v>
       </c>
@@ -3065,7 +3384,7 @@
       <c r="E33" s="6"/>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="9" t="s">
         <v>202</v>
       </c>
@@ -3076,7 +3395,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>7</v>
       </c>
@@ -3087,7 +3406,7 @@
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="9" t="s">
         <v>173</v>
       </c>
@@ -3098,7 +3417,7 @@
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="9" t="s">
         <v>183</v>
       </c>
@@ -3109,7 +3428,7 @@
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="9" t="s">
         <v>187</v>
       </c>
@@ -3120,7 +3439,7 @@
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>171</v>
       </c>
@@ -3131,7 +3450,7 @@
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>170</v>
       </c>
@@ -3142,7 +3461,7 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>125</v>
       </c>
@@ -3152,7 +3471,7 @@
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>126</v>
       </c>
@@ -3162,7 +3481,7 @@
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>112</v>
       </c>
@@ -3172,7 +3491,7 @@
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>209</v>
       </c>
@@ -3182,7 +3501,7 @@
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>161</v>
       </c>
@@ -3192,7 +3511,7 @@
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="9" t="s">
         <v>109</v>
       </c>
@@ -3203,7 +3522,7 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>102</v>
       </c>
@@ -3213,7 +3532,7 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>203</v>
       </c>
@@ -3223,7 +3542,7 @@
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>204</v>
       </c>
@@ -3233,7 +3552,7 @@
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>205</v>
       </c>
@@ -3243,7 +3562,7 @@
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>208</v>
       </c>
@@ -3253,7 +3572,7 @@
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="9" t="s">
         <v>206</v>
       </c>
@@ -3263,7 +3582,7 @@
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="9" t="s">
         <v>207</v>
       </c>
@@ -3272,7 +3591,7 @@
       </c>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="9" t="s">
         <v>105</v>
       </c>
@@ -3281,7 +3600,7 @@
       </c>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
         <v>117</v>
       </c>
@@ -3290,7 +3609,7 @@
       </c>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
         <v>124</v>
       </c>
@@ -3299,7 +3618,7 @@
       </c>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="9" t="s">
         <v>118</v>
       </c>
@@ -3308,7 +3627,7 @@
       </c>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
         <v>116</v>
       </c>
@@ -3317,7 +3636,7 @@
       </c>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
         <v>123</v>
       </c>
@@ -3326,7 +3645,7 @@
       </c>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>128</v>
       </c>
@@ -3335,7 +3654,7 @@
       </c>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
         <v>103</v>
       </c>
@@ -3344,7 +3663,7 @@
       </c>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
         <v>127</v>
       </c>
@@ -3353,7 +3672,7 @@
       </c>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
         <v>110</v>
       </c>
@@ -3362,7 +3681,7 @@
       </c>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
         <v>122</v>
       </c>
@@ -3371,7 +3690,7 @@
       </c>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
         <v>121</v>
       </c>
@@ -3380,7 +3699,7 @@
       </c>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
         <v>120</v>
       </c>
@@ -3389,7 +3708,7 @@
       </c>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
         <v>111</v>
       </c>
@@ -3398,7 +3717,7 @@
       </c>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
         <v>210</v>
       </c>
@@ -3407,7 +3726,7 @@
       </c>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="1:6">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
         <v>119</v>
       </c>
@@ -3416,7 +3735,7 @@
       </c>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
         <v>195</v>
       </c>
@@ -3426,7 +3745,7 @@
       <c r="D70" s="6"/>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="1:6">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="9" t="s">
         <v>104</v>
       </c>
@@ -3435,7 +3754,7 @@
       </c>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:6">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
         <v>211</v>
       </c>
@@ -3444,7 +3763,7 @@
       </c>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
         <v>19</v>
       </c>
@@ -3454,7 +3773,7 @@
       <c r="D73" s="6"/>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="9" t="s">
         <v>190</v>
       </c>
@@ -3464,7 +3783,7 @@
       <c r="D74" s="6"/>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:6">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="9" t="s">
         <v>189</v>
       </c>
@@ -3474,7 +3793,7 @@
       <c r="D75" s="6"/>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="1:6">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
         <v>213</v>
       </c>
@@ -3483,7 +3802,7 @@
       </c>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:6">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
         <v>214</v>
       </c>
@@ -3492,7 +3811,7 @@
       </c>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:6">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="9" t="s">
         <v>175</v>
       </c>
@@ -3502,7 +3821,7 @@
       <c r="D78" s="6"/>
       <c r="F78" s="6"/>
     </row>
-    <row r="79" spans="1:6">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="9" t="s">
         <v>177</v>
       </c>
@@ -3512,7 +3831,7 @@
       <c r="D79" s="6"/>
       <c r="F79" s="6"/>
     </row>
-    <row r="80" spans="1:6">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="9" t="s">
         <v>108</v>
       </c>
@@ -3521,7 +3840,7 @@
       </c>
       <c r="F80" s="6"/>
     </row>
-    <row r="81" spans="1:6">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
         <v>5</v>
       </c>
@@ -3531,7 +3850,7 @@
       <c r="D81" s="6"/>
       <c r="F81" s="6"/>
     </row>
-    <row r="82" spans="1:6">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="9" t="s">
         <v>20</v>
       </c>
@@ -3541,7 +3860,7 @@
       <c r="D82" s="6"/>
       <c r="F82" s="6"/>
     </row>
-    <row r="83" spans="1:6">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="9" t="s">
         <v>129</v>
       </c>
@@ -3550,7 +3869,7 @@
       </c>
       <c r="F83" s="6"/>
     </row>
-    <row r="84" spans="1:6">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="9" t="s">
         <v>114</v>
       </c>
@@ -3559,7 +3878,7 @@
       </c>
       <c r="F84" s="6"/>
     </row>
-    <row r="85" spans="1:6">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
         <v>113</v>
       </c>
@@ -3568,7 +3887,7 @@
       </c>
       <c r="F85" s="6"/>
     </row>
-    <row r="86" spans="1:6">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="9" t="s">
         <v>101</v>
       </c>
@@ -3577,7 +3896,7 @@
       </c>
       <c r="F86" s="6"/>
     </row>
-    <row r="87" spans="1:6">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="9" t="s">
         <v>218</v>
       </c>
@@ -3586,7 +3905,7 @@
       </c>
       <c r="F87" s="6"/>
     </row>
-    <row r="88" spans="1:6">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="9" t="s">
         <v>216</v>
       </c>
@@ -3595,7 +3914,7 @@
       </c>
       <c r="F88" s="6"/>
     </row>
-    <row r="89" spans="1:6">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="9" t="s">
         <v>212</v>
       </c>
@@ -3604,7 +3923,7 @@
       </c>
       <c r="F89" s="6"/>
     </row>
-    <row r="90" spans="1:6">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="9" t="s">
         <v>215</v>
       </c>
@@ -3613,7 +3932,7 @@
       </c>
       <c r="F90" s="6"/>
     </row>
-    <row r="91" spans="1:6">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="9" t="s">
         <v>17</v>
       </c>
@@ -3623,7 +3942,7 @@
       <c r="D91" s="6"/>
       <c r="F91" s="6"/>
     </row>
-    <row r="92" spans="1:6" s="6" customFormat="1">
+    <row r="92" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="7" t="s">
         <v>258</v>
       </c>
@@ -3632,7 +3951,7 @@
       </c>
       <c r="D92"/>
     </row>
-    <row r="93" spans="1:6">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="22" t="s">
         <v>248</v>
       </c>
@@ -3642,7 +3961,7 @@
       <c r="D93" s="6"/>
       <c r="F93" s="6"/>
     </row>
-    <row r="94" spans="1:6">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="9" t="s">
         <v>267</v>
       </c>
@@ -3650,7 +3969,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="95" spans="1:6">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="9" t="s">
         <v>269</v>
       </c>
@@ -3658,7 +3977,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="96" spans="1:6">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="9" t="s">
         <v>271</v>
       </c>
@@ -3666,7 +3985,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="9" t="s">
         <v>273</v>
       </c>
@@ -3674,7 +3993,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="9" t="s">
         <v>275</v>
       </c>
@@ -3682,7 +4001,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="9" t="s">
         <v>277</v>
       </c>
@@ -3690,7 +4009,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="9" t="s">
         <v>279</v>
       </c>
@@ -3698,7 +4017,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="9" t="s">
         <v>281</v>
       </c>
@@ -3706,7 +4025,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="s">
         <v>283</v>
       </c>
@@ -3714,7 +4033,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
         <v>285</v>
       </c>
@@ -3722,7 +4041,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="9" t="s">
         <v>287</v>
       </c>
@@ -3730,7 +4049,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="9" t="s">
         <v>289</v>
       </c>
@@ -3738,7 +4057,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="9" t="s">
         <v>295</v>
       </c>
@@ -3746,7 +4065,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="9" t="s">
         <v>291</v>
       </c>
@@ -3754,7 +4073,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="B109" s="13" t="s">
         <v>169</v>
       </c>
@@ -3770,11 +4089,6 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3786,13 +4100,13 @@
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="225.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="17" t="s">
         <v>228</v>
       </c>
@@ -3800,7 +4114,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>229</v>
       </c>
@@ -3808,7 +4122,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>230</v>
       </c>
@@ -3816,7 +4130,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>231</v>
       </c>
@@ -3824,7 +4138,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>244</v>
       </c>
@@ -3832,7 +4146,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>232</v>
       </c>
@@ -3840,7 +4154,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="18" t="s">
         <v>246</v>
       </c>
@@ -3848,7 +4162,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>233</v>
       </c>
@@ -3856,7 +4170,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>234</v>
       </c>
@@ -3864,7 +4178,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="28">
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>235</v>
       </c>
@@ -3872,11 +4186,11 @@
         <v>241</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="20"/>
       <c r="B11" s="20"/>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="20"/>
       <c r="B12" s="21"/>
     </row>
@@ -3884,10 +4198,5 @@
   <autoFilter ref="A1:B10"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>